<commit_message>
Redesign libro diario read algorithm
</commit_message>
<xml_diff>
--- a/libroDiario.xlsx
+++ b/libroDiario.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
   <si>
     <t>Libro Diario</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>IVA</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
   <si>
     <t>Capital</t>
@@ -224,10 +227,12 @@
       <c r="E4" s="3"/>
     </row>
     <row r="5">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3">
@@ -236,18 +241,18 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3">
@@ -256,10 +261,12 @@
       <c r="E7" s="3"/>
     </row>
     <row r="8">
-      <c r="A8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3">
@@ -268,18 +275,18 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3">
@@ -288,10 +295,12 @@
       <c r="E10" s="3"/>
     </row>
     <row r="11">
-      <c r="A11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3">
@@ -302,7 +311,7 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3">
@@ -311,15 +320,15 @@
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>6</v>
@@ -344,7 +353,7 @@
     <row r="16">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3">
@@ -355,7 +364,7 @@
     <row r="17">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3">
@@ -366,7 +375,7 @@
     <row r="18">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3">
@@ -375,10 +384,12 @@
       <c r="E18" s="3"/>
     </row>
     <row r="19">
-      <c r="A19" s="3"/>
+      <c r="A19" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3">
@@ -387,18 +398,18 @@
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3">
@@ -407,10 +418,12 @@
       <c r="E21" s="3"/>
     </row>
     <row r="22">
-      <c r="A22" s="3"/>
+      <c r="A22" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3">
@@ -419,10 +432,10 @@
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24">
@@ -454,10 +467,10 @@
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3">
@@ -466,10 +479,12 @@
       <c r="E28" s="3"/>
     </row>
     <row r="29">
-      <c r="A29" s="3"/>
+      <c r="A29" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3">
@@ -478,10 +493,10 @@
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31">
@@ -509,10 +524,12 @@
       <c r="E32" s="3"/>
     </row>
     <row r="33">
-      <c r="A33" s="3"/>
+      <c r="A33" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3">
@@ -521,18 +538,18 @@
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3">
@@ -541,7 +558,9 @@
       <c r="E35" s="3"/>
     </row>
     <row r="36">
-      <c r="A36" s="3"/>
+      <c r="A36" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
         <v>6</v>
@@ -555,7 +574,7 @@
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E37" s="3">
         <v>343434.0</v>
@@ -563,10 +582,10 @@
     </row>
     <row r="38">
       <c r="A38" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C38" s="3"/>
       <c r="E38" s="3"/>

</xml_diff>